<commit_message>
quiero que vuelvan las canciones brasileras del 2014
</commit_message>
<xml_diff>
--- a/TP4/Ejercicio-2/Cálculos.xlsx
+++ b/TP4/Ejercicio-2/Cálculos.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\germa\Documents\GitHub\LABO\TP4\Ejercicio-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EBE628-80BF-45E9-A28B-B4BA98101641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64270F8-B085-45D8-9011-497CA85C5D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{150D0140-DD95-49BE-91AF-880EEFCE36FC}"/>
   </bookViews>
   <sheets>
-    <sheet name="R=16K" sheetId="2" r:id="rId1"/>
+    <sheet name="R" sheetId="2" r:id="rId1"/>
     <sheet name="R=K795" sheetId="1" state="hidden" r:id="rId2"/>
     <sheet name="R=8K" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="b) Error" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>f[Hz]</t>
   </si>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F81C4A-4B2E-4256-A411-1C957A1CC369}">
-  <dimension ref="C1:L47"/>
+  <dimension ref="C1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,9 +486,6 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
@@ -540,33 +537,40 @@
         <v>15000</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D41" si="0">$H$2*$K$2*ABS((2*PI()*C3*$J$2*I3)/((2*PI()*C3*$J$2*I3)+1))*$L$2</f>
+        <f t="shared" ref="D3:D40" si="0">$H$2*$K$2*ABS((2*PI()*C3*$J$2*I3)/((2*PI()*C3*$J$2*I3)+1))*$L$2</f>
         <v>1.111E-2</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E41" si="1">$H$2*$K$2*ABS(((2*PI()*C3*$J$2*I3)+1))*$L$2</f>
+        <f t="shared" ref="E3:E40" si="1">$H$2*$K$2*ABS(((2*PI()*C3*$J$2*I3)+1))*$L$2</f>
         <v>4.444E-2</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I41" si="2">1/(2*PI()*C3*$J$2)</f>
+        <f t="shared" ref="I3:I40" si="2">1/(2*PI()*C3*$J$2)</f>
         <v>10610.32953945969</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" s="1">
-        <v>65010</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+        <f>C3+5000</f>
+        <v>20000</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.111E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="1"/>
+        <v>4.444E-2</v>
+      </c>
       <c r="I4" s="3">
         <f t="shared" si="2"/>
-        <v>2448.1609458836383</v>
+        <v>7957.7471545947665</v>
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
-        <f>C3+5000</f>
-        <v>20000</v>
+        <f t="shared" ref="C5:C40" si="3">C4+5000</f>
+        <v>25000</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
@@ -578,13 +582,13 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" si="2"/>
-        <v>7957.7471545947665</v>
+        <v>6366.1977236758139</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C41" si="3">C5+5000</f>
-        <v>25000</v>
+        <f t="shared" si="3"/>
+        <v>30000</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
@@ -596,17 +600,17 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" si="2"/>
-        <v>6366.1977236758139</v>
+        <v>5305.1647697298449</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <f t="shared" si="3"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
@@ -614,17 +618,17 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" si="2"/>
-        <v>5305.1647697298449</v>
+        <v>4547.2840883398667</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f t="shared" si="3"/>
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
@@ -632,13 +636,13 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" si="2"/>
-        <v>4547.2840883398667</v>
+        <v>3978.8735772973832</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f t="shared" si="3"/>
-        <v>40000</v>
+        <v>45000</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
@@ -650,13 +654,13 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" si="2"/>
-        <v>3978.8735772973832</v>
+        <v>3536.7765131532292</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f t="shared" si="3"/>
-        <v>45000</v>
+        <v>50000</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
@@ -668,17 +672,17 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="2"/>
-        <v>3536.7765131532292</v>
+        <v>3183.098861837907</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <f t="shared" si="3"/>
-        <v>50000</v>
+        <v>55000</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
@@ -686,17 +690,17 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" si="2"/>
-        <v>3183.098861837907</v>
+        <v>2893.7262380344605</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <f t="shared" si="3"/>
-        <v>55000</v>
+        <v>60000</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
@@ -704,17 +708,17 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" si="2"/>
-        <v>2893.7262380344605</v>
+        <v>2652.5823848649225</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <f t="shared" si="3"/>
-        <v>60000</v>
+        <v>65000</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
@@ -722,13 +726,13 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" si="2"/>
-        <v>2652.5823848649225</v>
+        <v>2448.5375860291588</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <f t="shared" si="3"/>
-        <v>65000</v>
+        <v>70000</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
@@ -740,13 +744,13 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" si="2"/>
-        <v>2448.5375860291588</v>
+        <v>2273.6420441699333</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <f t="shared" si="3"/>
-        <v>70000</v>
+        <v>75000</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="0"/>
@@ -758,17 +762,17 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" si="2"/>
-        <v>2273.6420441699333</v>
+        <v>2122.0659078919375</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <f t="shared" si="3"/>
-        <v>75000</v>
+        <v>80000</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
@@ -776,13 +780,13 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" si="2"/>
-        <v>2122.0659078919375</v>
+        <v>1989.4367886486916</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <f t="shared" si="3"/>
-        <v>80000</v>
+        <v>85000</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="0"/>
@@ -794,13 +798,13 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" si="2"/>
-        <v>1989.4367886486916</v>
+        <v>1872.4110951987689</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <f t="shared" si="3"/>
-        <v>85000</v>
+        <v>90000</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
@@ -812,13 +816,13 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" si="2"/>
-        <v>1872.4110951987689</v>
+        <v>1768.3882565766146</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <f t="shared" si="3"/>
-        <v>90000</v>
+        <v>95000</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
@@ -830,13 +834,13 @@
       </c>
       <c r="I19" s="3">
         <f t="shared" si="2"/>
-        <v>1768.3882565766146</v>
+        <v>1675.3151904410036</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <f t="shared" si="3"/>
-        <v>95000</v>
+        <v>100000</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="0"/>
@@ -848,13 +852,13 @@
       </c>
       <c r="I20" s="3">
         <f t="shared" si="2"/>
-        <v>1675.3151904410036</v>
+        <v>1591.5494309189535</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <f t="shared" si="3"/>
-        <v>100000</v>
+        <v>105000</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
@@ -866,17 +870,17 @@
       </c>
       <c r="I21" s="3">
         <f t="shared" si="2"/>
-        <v>1591.5494309189535</v>
+        <v>1515.7613627799553</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <f t="shared" si="3"/>
-        <v>105000</v>
+        <v>110000</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
@@ -884,17 +888,17 @@
       </c>
       <c r="I22" s="3">
         <f t="shared" si="2"/>
-        <v>1515.7613627799553</v>
+        <v>1446.8631190172302</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <f t="shared" si="3"/>
-        <v>110000</v>
+        <v>115000</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
@@ -902,13 +906,13 @@
       </c>
       <c r="I23" s="3">
         <f t="shared" si="2"/>
-        <v>1446.8631190172302</v>
+        <v>1383.9560268860464</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <f t="shared" si="3"/>
-        <v>115000</v>
+        <v>120000</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="0"/>
@@ -920,17 +924,17 @@
       </c>
       <c r="I24" s="3">
         <f t="shared" si="2"/>
-        <v>1383.9560268860464</v>
+        <v>1326.2911924324612</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <f t="shared" si="3"/>
-        <v>120000</v>
+        <v>125000</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="1"/>
@@ -938,13 +942,13 @@
       </c>
       <c r="I25" s="3">
         <f t="shared" si="2"/>
-        <v>1326.2911924324612</v>
+        <v>1273.2395447351626</v>
       </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <f t="shared" si="3"/>
-        <v>125000</v>
+        <v>130000</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="0"/>
@@ -956,17 +960,17 @@
       </c>
       <c r="I26" s="3">
         <f t="shared" si="2"/>
-        <v>1273.2395447351626</v>
+        <v>1224.2687930145794</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <f t="shared" si="3"/>
-        <v>130000</v>
+        <v>135000</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
@@ -974,17 +978,17 @@
       </c>
       <c r="I27" s="3">
         <f t="shared" si="2"/>
-        <v>1224.2687930145794</v>
+        <v>1178.9255043844098</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <f t="shared" si="3"/>
-        <v>135000</v>
+        <v>140000</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
@@ -992,17 +996,17 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" si="2"/>
-        <v>1178.9255043844098</v>
+        <v>1136.8210220849667</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <f t="shared" si="3"/>
-        <v>140000</v>
+        <v>145000</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
@@ -1010,17 +1014,17 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" si="2"/>
-        <v>1136.8210220849667</v>
+        <v>1097.620297185485</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <f t="shared" si="3"/>
-        <v>145000</v>
+        <v>150000</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
@@ -1028,17 +1032,17 @@
       </c>
       <c r="I30" s="3">
         <f t="shared" si="2"/>
-        <v>1097.620297185485</v>
+        <v>1061.0329539459688</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <f t="shared" si="3"/>
-        <v>150000</v>
+        <v>155000</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
@@ -1046,13 +1050,13 @@
       </c>
       <c r="I31" s="3">
         <f t="shared" si="2"/>
-        <v>1061.0329539459688</v>
+        <v>1026.806084463841</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <f t="shared" si="3"/>
-        <v>155000</v>
+        <v>160000</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="0"/>
@@ -1064,13 +1068,13 @@
       </c>
       <c r="I32" s="3">
         <f t="shared" si="2"/>
-        <v>1026.806084463841</v>
+        <v>994.71839432434581</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <f t="shared" si="3"/>
-        <v>160000</v>
+        <v>165000</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="0"/>
@@ -1082,13 +1086,13 @@
       </c>
       <c r="I33" s="3">
         <f t="shared" si="2"/>
-        <v>994.71839432434581</v>
+        <v>964.57541267815361</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <f t="shared" si="3"/>
-        <v>165000</v>
+        <v>170000</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="0"/>
@@ -1100,13 +1104,13 @@
       </c>
       <c r="I34" s="3">
         <f t="shared" si="2"/>
-        <v>964.57541267815361</v>
+        <v>936.20554759938443</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <f t="shared" si="3"/>
-        <v>170000</v>
+        <v>175000</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="0"/>
@@ -1118,13 +1122,13 @@
       </c>
       <c r="I35" s="3">
         <f t="shared" si="2"/>
-        <v>936.20554759938443</v>
+        <v>909.45681766797338</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <f t="shared" si="3"/>
-        <v>175000</v>
+        <v>180000</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="0"/>
@@ -1136,13 +1140,13 @@
       </c>
       <c r="I36" s="3">
         <f t="shared" si="2"/>
-        <v>909.45681766797338</v>
+        <v>884.1941282883073</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <f t="shared" si="3"/>
-        <v>180000</v>
+        <v>185000</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="0"/>
@@ -1154,13 +1158,13 @@
       </c>
       <c r="I37" s="3">
         <f t="shared" si="2"/>
-        <v>884.1941282883073</v>
+        <v>860.29698968592072</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <f t="shared" si="3"/>
-        <v>185000</v>
+        <v>190000</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="0"/>
@@ -1172,17 +1176,17 @@
       </c>
       <c r="I38" s="3">
         <f t="shared" si="2"/>
-        <v>860.29698968592072</v>
+        <v>837.65759522050178</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <f t="shared" si="3"/>
-        <v>190000</v>
+        <v>195000</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="0"/>
-        <v>1.111E-2</v>
+        <v>1.1109999999999998E-2</v>
       </c>
       <c r="E39" s="4">
         <f t="shared" si="1"/>
@@ -1190,17 +1194,17 @@
       </c>
       <c r="I39" s="3">
         <f t="shared" si="2"/>
-        <v>837.65759522050178</v>
+        <v>816.17919534305292</v>
       </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f t="shared" si="3"/>
-        <v>195000</v>
+        <v>200000</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="0"/>
-        <v>1.1109999999999998E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" si="1"/>
@@ -1208,26 +1212,11 @@
       </c>
       <c r="I40" s="3">
         <f t="shared" si="2"/>
-        <v>816.17919534305292</v>
+        <v>795.77471545947674</v>
       </c>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="1">
-        <f t="shared" si="3"/>
-        <v>200000</v>
-      </c>
-      <c r="D41" s="4">
-        <f t="shared" si="0"/>
-        <v>1.111E-2</v>
-      </c>
-      <c r="E41" s="4">
-        <f t="shared" si="1"/>
-        <v>4.444E-2</v>
-      </c>
-      <c r="I41" s="3">
-        <f t="shared" si="2"/>
-        <v>795.77471545947674</v>
-      </c>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
@@ -1243,9 +1232,6 @@
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2470,7 +2456,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2479,7 +2465,7 @@
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -2529,11 +2515,11 @@
         <v>7.95</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D7" si="0">1/(SQRT(B3*C3*1000000)*2*PI()*0.000000001)/1000</f>
+        <f t="shared" ref="D3:D4" si="0">1/(SQRT(B3*C3*1000000)*2*PI()*0.000000001)/1000</f>
         <v>20.570226758119215</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="E3:E7" si="1">ABS(A3-D3)*100/A3</f>
+        <f t="shared" ref="E3:E4" si="1">ABS(A3-D3)*100/A3</f>
         <v>2.6952376626337995</v>
       </c>
     </row>
@@ -2658,6 +2644,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <f>AVERAGE(E2:E9)</f>
+        <v>1.9744490499396667</v>
+      </c>
       <c r="O10" t="s">
         <v>11</v>
       </c>

</xml_diff>